<commit_message>
questions and answers are completed
</commit_message>
<xml_diff>
--- a/Data/HIV-chatbot-data.xlsx
+++ b/Data/HIV-chatbot-data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4be00a87f5d1ad95/Documents/chatbot-HIV/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4be00a87f5d1ad95/Documents/chatbot-HIV/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_58A465B6D5703C8E53CD4CCDA79FF9ACB9203C6B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D1EA0FA1-2002-4BB4-9D9A-876F1C393EAF}"/>
+  <xr:revisionPtr revIDLastSave="85" documentId="11_58A465B6D5703C8E53CD4CCDA79FF9ACB9203C6B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E0DE6D43-A0A6-4540-8901-9E1A3B33D2C2}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,101 +20,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
-  <si>
-    <t xml:space="preserve">       Q1                                                            A1</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="41">
   <si>
     <t xml:space="preserve">Can HIV be cured?                                        </t>
   </si>
   <si>
-    <t xml:space="preserve">What is the cure for HIV?                       Currently, there is no permanent cure for HIV yet, </t>
-  </si>
-  <si>
-    <t xml:space="preserve">What drug can be used to cure HIV?              Some combination of drugs known as Anti retroviral therapy are used for treatment.     </t>
-  </si>
-  <si>
-    <t>Does HIV have a cure?                           They act by reducing the viral load.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     Q2                                                              A2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">What is antiretroval therapy?                   HIV can be treated, but not permanently cured with antiretroviral therapy(ART). </t>
-  </si>
-  <si>
-    <t>What is ART                                     These combination of drugs act by reducing the HIV viral load, with this, the patient</t>
-  </si>
-  <si>
-    <t>What drug can a HIV positive person take?       can live a normal life without symptoms and can also not be able to transmit</t>
-  </si>
-  <si>
-    <t>What is drug of choice for HIV                  the virus.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     Q3                                                              A3</t>
-  </si>
-  <si>
-    <t>What is PrEP?                                   Pre-exposure prophylaxis (PrEP) is medicine people at risk for HIV take to prevent getting HIV</t>
-  </si>
-  <si>
-    <t>What is pre-exposure prophylaxis?               from sex or drug use. PrEP is taken before exposure</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     Q4                                                              A4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">What is PEP?                                    Post-exposure prophylaxis(PEP) is a HIV prevention drug taken by people who are already exposed </t>
-  </si>
-  <si>
-    <t>What is Post-exposure prophylaxis?              to HIV, Ideally its taken within 72 hours of exposure. PEP is taken after exposure.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     Q5                                                              A5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Can HIV be prevented with drugs?                HIV can be prevented just before and after exposure by some classes of drugs known as PrEP and </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Is there any immunization for HIV?              PEP respectively. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">     Q6                                                              A6</t>
-  </si>
-  <si>
-    <t>How do I get on HIV treatment?                  Once you are diagnosed of HIV, make an appointment to see a health care provider about starting</t>
-  </si>
-  <si>
-    <t>How do I start treating HIV?                    HIV treatment. Don't wait until you feel sick. They will recomment the best combination therapy</t>
-  </si>
-  <si>
-    <t>Recommend best HIV treatment for me             /ART for you spacifically</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      Q7                                                             A7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">How long is HIV treatment                       Since HIV cannot be cured for now, The available combination therapies are meant to be taken for </t>
-  </si>
-  <si>
-    <t>what is the dose of HIV drug                    a lifetime inorder to suppress the viral load to the minimal level. These therapies can come inform</t>
-  </si>
-  <si>
-    <t>How do I take the HIV drug?                     of a monthly injection, once or multiple times daily.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      Q8                                                             A8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">How can I access a HIV drug?                    Antiretroviral drugs used for treating HIV are prescription drugs ideally. To access them, one has to </t>
-  </si>
-  <si>
-    <t xml:space="preserve">How do I start HIV treatment?                   have a Doctor's prescription. This is because ARV treatment regimen differs for different individual.  </t>
-  </si>
-  <si>
-    <t>How accessible is HIV drug?                     So it is adviced to always visit the hospital for ARV prescription and collection</t>
-  </si>
-  <si>
     <t xml:space="preserve">Do I need prescription to buy HIV drug? </t>
   </si>
   <si>
@@ -125,18 +35,133 @@
   </si>
   <si>
     <t xml:space="preserve">      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">What is the cure for HIV?                        </t>
+  </si>
+  <si>
+    <t>Currently, there is no permanent cure for HIV yet,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What drug can be used to cure HIV?                   </t>
+  </si>
+  <si>
+    <t>Some combination of drugs known as Anti retroviral therapy are used for treatment.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Does HIV have a cure?                           </t>
+  </si>
+  <si>
+    <t>They act by reducing the viral load.</t>
+  </si>
+  <si>
+    <t>Currently, there is no permanent cure for HIV.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What is antiretroval therapy?                    </t>
+  </si>
+  <si>
+    <t>HIV can be treated, but not permanently cured with antiretroviral therapy(ART).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What is ART                                     </t>
+  </si>
+  <si>
+    <t>What drug can a HIV positive person take?</t>
+  </si>
+  <si>
+    <t>What is drug of choice for HIV</t>
+  </si>
+  <si>
+    <t>question</t>
+  </si>
+  <si>
+    <t>answer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What is PrEP?                                   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">What is pre-exposure prophylaxis?               </t>
+  </si>
+  <si>
+    <t>Pre-exposure prophylaxis (PrEP) is medicine people at risk for HIV take to prevent getting HIV from sex or drug use. PrEP is taken before exposure</t>
+  </si>
+  <si>
+    <t>These combination of drugs act by reducing the HIV viral load, with this, the patient can live a normal life without symptoms and can also not be able to transmit the virus.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What is PEP?                                     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">What is Post-exposure prophylaxis?              </t>
+  </si>
+  <si>
+    <t>Post-exposure prophylaxis(PEP) is a HIV prevention drug taken by people who are already exposed to HIV, Ideally its taken within 72 hours of exposure. PEP is taken after exposure.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Can HIV be prevented with drugs? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">HIV can be prevented just before and after exposure by some classes of drugs known as PrEP and PEP respectively. </t>
+  </si>
+  <si>
+    <t>Is there any immunization for HIV?</t>
+  </si>
+  <si>
+    <t>How do I get on HIV treatment?</t>
+  </si>
+  <si>
+    <t>Once you are diagnosed of HIV, make an appointment to see a health care provider about starting HIV treatment. Don't wait until you feel sick. They will recomment the best combination therapy  /ART for you spacifically</t>
+  </si>
+  <si>
+    <t>Recommend best HIV treatment for me</t>
+  </si>
+  <si>
+    <t>How do I start treating HIV?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How long is HIV treatment                       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">what is the dose of HIV drug                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">How do I take the HIV drug?                     </t>
+  </si>
+  <si>
+    <t>Since HIV cannot be cured for now, The available combination therapies are meant to be taken for a lifetime inorder to suppress the viral load to the minimal level. These therapies can come inform of a monthly injection, once or multiple times daily.</t>
+  </si>
+  <si>
+    <t>How can I access a HIV drug?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How do I start HIV treatment?                     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">How accessible is HIV drug?                     </t>
+  </si>
+  <si>
+    <t>Antiretroviral drugs used for treating HIV are prescription drugs ideally. To access them, one has to have a Doctor's prescription. This is because ARV treatment regimen differs for different individual.So it is adviced to always visit the hospital for ARV prescription and collection.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -162,8 +187,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -658,187 +686,230 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A43"/>
+  <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.77734375" defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="117.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
+      <c r="B25" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
-      <c r="A4" t="s">
+    <row r="32" spans="1:2">
+      <c r="A32" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1">
-      <c r="A11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1">
-      <c r="A12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1">
-      <c r="A13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1">
-      <c r="A14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1">
-      <c r="A15" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1">
-      <c r="A16" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1">
-      <c r="A19" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1">
-      <c r="A20" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1">
-      <c r="A21" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1">
-      <c r="A22" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1">
-      <c r="A23" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1">
-      <c r="A24" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1">
-      <c r="A25" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1">
-      <c r="A26" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1">
-      <c r="A27" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1">
-      <c r="A28" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1">
-      <c r="A30" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1">
-      <c r="A31" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1">
-      <c r="A32" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1">
-      <c r="A33" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1">
-      <c r="A38" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1">
-      <c r="A41" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1">
-      <c r="A43" t="s">
-        <v>34</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>